<commit_message>
Update SARSA file for bet_sizing
</commit_message>
<xml_diff>
--- a/results_cmp.xlsx
+++ b/results_cmp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yixiang/repos/cs4246-project-blackjack/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\cs4246-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9061B683-D702-4A4D-857B-1850E9AF5EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D7BCDC-B0EF-44D6-8342-334E192977BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="17340" windowHeight="18900" xr2:uid="{055D1B8C-A1B7-2E42-AC74-8FEFC4B03BAD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{055D1B8C-A1B7-2E42-AC74-8FEFC4B03BAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimal preplay ep" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Preplay episodes</t>
   </si>
@@ -86,6 +86,21 @@
   </si>
   <si>
     <t>pending</t>
+  </si>
+  <si>
+    <t>pending full info also</t>
+  </si>
+  <si>
+    <t>all of these are saved into full info</t>
+  </si>
+  <si>
+    <t>only 100_100 belongs to full info</t>
+  </si>
+  <si>
+    <t>transfer the rest into add split</t>
+  </si>
+  <si>
+    <t>need to run bet sizing sarsa file</t>
   </si>
 </sst>
 </file>
@@ -458,18 +473,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA56301A-5BE6-A148-9F15-753DAC43EA57}">
-  <dimension ref="B1:E8"/>
+  <dimension ref="B1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1000000</v>
       </c>
@@ -490,8 +505,11 @@
       <c r="E2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>5000000</v>
       </c>
@@ -501,8 +519,11 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>20000000</v>
       </c>
@@ -512,16 +533,25 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>50000000</v>
       </c>
       <c r="C5" s="1">
         <v>50000000</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>100000000</v>
       </c>
@@ -532,20 +562,26 @@
         <v>4.6349999999999999E-4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>200000000</v>
       </c>
       <c r="C7" s="1">
         <v>50000000</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>500000000</v>
       </c>
       <c r="C8" s="1">
         <v>50000000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -561,9 +597,9 @@
       <selection activeCell="B1" sqref="B1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -585,7 +621,7 @@
         <v>-2.2980000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -596,7 +632,7 @@
         <v>4.6349999999999999E-4</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -607,7 +643,7 @@
         <v>8.5349999999999998E-4</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -618,7 +654,7 @@
         <v>-2.1679999999999998E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -630,18 +666,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB12773-D184-3748-80F7-005D7C1CBB85}">
-  <dimension ref="B1:E5"/>
+  <dimension ref="B1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -655,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -665,8 +701,11 @@
       <c r="D2" s="1">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -676,8 +715,11 @@
       <c r="D3" s="1">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -687,8 +729,11 @@
       <c r="D4" s="1">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>

</xml_diff>